<commit_message>
Refactor code, implement activities, begin unit tests
</commit_message>
<xml_diff>
--- a/Fonctionalités Trello.xlsx
+++ b/Fonctionalités Trello.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{DCB8761E-D25A-4083-84B0-6B2C38CAB824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C99E2E28-7B48-4DE1-98F6-96BE9FB3E847}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{DCB8761E-D25A-4083-84B0-6B2C38CAB824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87699293-CB27-4D10-A7C9-B950BAAE7C23}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>37</v>
@@ -600,7 +600,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>37</v>
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>37</v>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>37</v>
@@ -642,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>37</v>
@@ -656,7 +656,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>37</v>
@@ -754,7 +754,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Make SprintMenu drag'n'drop multitouch + doc restruct
</commit_message>
<xml_diff>
--- a/Fonctionalités Trello.xlsx
+++ b/Fonctionalités Trello.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{DCB8761E-D25A-4083-84B0-6B2C38CAB824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87699293-CB27-4D10-A7C9-B950BAAE7C23}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{DCB8761E-D25A-4083-84B0-6B2C38CAB824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5D14866-893C-4102-B311-8AE03BAE231E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12555" yWindow="2865" windowWidth="18975" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -164,15 +164,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,16 +186,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -413,358 +437,358 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="102.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1"/>
-    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="14.42578125" style="1"/>
+    <col min="1" max="1" width="102.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2"/>
+    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="D20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="D22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>